<commit_message>
Fix clinical breakpoint seed
- Wrong enum value for CLSI
- Missing ValidFrom data
- Missing "No-Specific" species entries

#2
</commit_message>
<xml_diff>
--- a/Documents/clinical-breakpoints.xlsx
+++ b/Documents/clinical-breakpoints.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Development\NRZMyk\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D8BC96E2-C529-4B11-88B8-006AA158354B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{216C4A79-C8FA-43DB-9363-6996D69C7FE8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30" yWindow="780" windowWidth="28770" windowHeight="15270" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Breakpoints EUCAST and CLSI" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1478" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1542" uniqueCount="109">
   <si>
     <t>Amphotericin B</t>
   </si>
@@ -291,9 +291,6 @@
     <t>0.001</t>
   </si>
   <si>
-    <t>Non-species specific</t>
-  </si>
-  <si>
     <t>Isavuconazole</t>
   </si>
   <si>
@@ -352,6 +349,12 @@
   </si>
   <si>
     <t>MicBreakpointResistent</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>2019-11-01</t>
   </si>
 </sst>
 </file>
@@ -725,14 +728,17 @@
   <dimension ref="A1:J129"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="21.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="25.85546875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="19.7109375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="22.42578125" bestFit="1" customWidth="1"/>
@@ -741,7 +747,7 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>3</v>
@@ -753,30 +759,30 @@
         <v>6</v>
       </c>
       <c r="E1" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="F1" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="G1" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="H1" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="I1" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="I1" s="4" t="s">
-        <v>107</v>
-      </c>
       <c r="J1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C2" s="6" t="s">
         <v>5</v>
@@ -801,10 +807,10 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C3" s="6" t="s">
         <v>5</v>
@@ -829,10 +835,10 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C4" s="6" t="s">
         <v>5</v>
@@ -857,10 +863,10 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B5" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C5" s="6" t="s">
         <v>5</v>
@@ -881,10 +887,10 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B6" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C6" s="6" t="s">
         <v>5</v>
@@ -909,10 +915,10 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C7" s="6" t="s">
         <v>5</v>
@@ -937,10 +943,10 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B8" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C8" s="6" t="s">
         <v>5</v>
@@ -968,7 +974,7 @@
         <v>45</v>
       </c>
       <c r="B9" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C9" s="6" t="s">
         <v>5</v>
@@ -996,7 +1002,7 @@
         <v>45</v>
       </c>
       <c r="B10" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C10" s="6" t="s">
         <v>5</v>
@@ -1020,7 +1026,7 @@
         <v>45</v>
       </c>
       <c r="B11" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C11" s="6" t="s">
         <v>5</v>
@@ -1048,7 +1054,7 @@
         <v>45</v>
       </c>
       <c r="B12" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C12" s="6" t="s">
         <v>5</v>
@@ -1072,7 +1078,7 @@
         <v>45</v>
       </c>
       <c r="B13" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C13" s="6" t="s">
         <v>5</v>
@@ -1100,7 +1106,7 @@
         <v>45</v>
       </c>
       <c r="B14" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C14" s="6" t="s">
         <v>5</v>
@@ -1128,7 +1134,7 @@
         <v>45</v>
       </c>
       <c r="B15" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C15" s="6" t="s">
         <v>5</v>
@@ -1156,7 +1162,7 @@
         <v>47</v>
       </c>
       <c r="B16" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C16" s="6" t="s">
         <v>5</v>
@@ -1180,7 +1186,7 @@
         <v>47</v>
       </c>
       <c r="B17" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C17" s="6" t="s">
         <v>5</v>
@@ -1204,7 +1210,7 @@
         <v>47</v>
       </c>
       <c r="B18" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C18" s="6" t="s">
         <v>5</v>
@@ -1228,7 +1234,7 @@
         <v>47</v>
       </c>
       <c r="B19" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C19" s="6" t="s">
         <v>5</v>
@@ -1252,7 +1258,7 @@
         <v>47</v>
       </c>
       <c r="B20" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C20" s="6" t="s">
         <v>5</v>
@@ -1276,7 +1282,7 @@
         <v>47</v>
       </c>
       <c r="B21" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C21" s="6" t="s">
         <v>5</v>
@@ -1300,7 +1306,7 @@
         <v>47</v>
       </c>
       <c r="B22" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C22" s="6" t="s">
         <v>5</v>
@@ -1324,7 +1330,7 @@
         <v>48</v>
       </c>
       <c r="B23" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C23" s="6" t="s">
         <v>5</v>
@@ -1354,7 +1360,7 @@
         <v>48</v>
       </c>
       <c r="B24" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C24" s="6" t="s">
         <v>5</v>
@@ -1378,7 +1384,7 @@
         <v>48</v>
       </c>
       <c r="B25" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C25" s="6" t="s">
         <v>5</v>
@@ -1406,7 +1412,7 @@
         <v>48</v>
       </c>
       <c r="B26" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C26" s="6" t="s">
         <v>5</v>
@@ -1430,7 +1436,7 @@
         <v>48</v>
       </c>
       <c r="B27" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C27" s="6" t="s">
         <v>5</v>
@@ -1454,7 +1460,7 @@
         <v>48</v>
       </c>
       <c r="B28" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C28" s="6" t="s">
         <v>5</v>
@@ -1482,7 +1488,7 @@
         <v>48</v>
       </c>
       <c r="B29" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C29" s="6" t="s">
         <v>5</v>
@@ -1506,7 +1512,7 @@
         <v>49</v>
       </c>
       <c r="B30" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C30" s="6" t="s">
         <v>5</v>
@@ -1534,7 +1540,7 @@
         <v>49</v>
       </c>
       <c r="B31" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C31" s="6" t="s">
         <v>5</v>
@@ -1562,7 +1568,7 @@
         <v>49</v>
       </c>
       <c r="B32" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C32" s="6" t="s">
         <v>5</v>
@@ -1586,7 +1592,7 @@
         <v>49</v>
       </c>
       <c r="B33" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C33" s="6" t="s">
         <v>5</v>
@@ -1610,7 +1616,7 @@
         <v>49</v>
       </c>
       <c r="B34" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C34" s="6" t="s">
         <v>5</v>
@@ -1634,7 +1640,7 @@
         <v>49</v>
       </c>
       <c r="B35" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C35" s="6" t="s">
         <v>5</v>
@@ -1662,7 +1668,7 @@
         <v>49</v>
       </c>
       <c r="B36" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C36" s="6" t="s">
         <v>5</v>
@@ -1690,7 +1696,7 @@
         <v>50</v>
       </c>
       <c r="B37" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C37" s="6" t="s">
         <v>5</v>
@@ -1718,7 +1724,7 @@
         <v>50</v>
       </c>
       <c r="B38" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C38" s="6" t="s">
         <v>5</v>
@@ -1746,7 +1752,7 @@
         <v>50</v>
       </c>
       <c r="B39" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C39" s="6" t="s">
         <v>5</v>
@@ -1774,7 +1780,7 @@
         <v>50</v>
       </c>
       <c r="B40" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C40" s="6" t="s">
         <v>5</v>
@@ -1798,7 +1804,7 @@
         <v>50</v>
       </c>
       <c r="B41" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C41" s="6" t="s">
         <v>5</v>
@@ -1822,7 +1828,7 @@
         <v>50</v>
       </c>
       <c r="B42" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C42" s="6" t="s">
         <v>5</v>
@@ -1850,7 +1856,7 @@
         <v>50</v>
       </c>
       <c r="B43" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C43" s="6" t="s">
         <v>5</v>
@@ -1878,7 +1884,7 @@
         <v>50</v>
       </c>
       <c r="B44" t="s">
-        <v>87</v>
+        <v>107</v>
       </c>
       <c r="C44" s="6" t="s">
         <v>5</v>
@@ -1903,10 +1909,10 @@
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B45" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C45" s="6" t="s">
         <v>5</v>
@@ -1922,15 +1928,15 @@
       <c r="H45" s="2"/>
       <c r="I45" s="2"/>
       <c r="J45" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B46" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C46" s="6" t="s">
         <v>5</v>
@@ -1946,15 +1952,15 @@
       <c r="H46" s="2"/>
       <c r="I46" s="2"/>
       <c r="J46" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B47" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C47" s="6" t="s">
         <v>5</v>
@@ -1970,15 +1976,15 @@
       <c r="H47" s="2"/>
       <c r="I47" s="2"/>
       <c r="J47" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B48" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C48" s="6" t="s">
         <v>5</v>
@@ -1994,15 +2000,15 @@
       <c r="H48" s="2"/>
       <c r="I48" s="2"/>
       <c r="J48" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B49" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C49" s="6" t="s">
         <v>5</v>
@@ -2018,15 +2024,15 @@
       <c r="H49" s="2"/>
       <c r="I49" s="2"/>
       <c r="J49" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B50" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C50" s="6" t="s">
         <v>5</v>
@@ -2042,15 +2048,15 @@
       <c r="H50" s="2"/>
       <c r="I50" s="2"/>
       <c r="J50" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B51" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C51" s="6" t="s">
         <v>5</v>
@@ -2066,15 +2072,15 @@
       <c r="H51" s="2"/>
       <c r="I51" s="2"/>
       <c r="J51" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B52" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C52" s="6" t="s">
         <v>5</v>
@@ -2094,15 +2100,15 @@
         <v>83</v>
       </c>
       <c r="J52" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B53" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C53" s="6" t="s">
         <v>5</v>
@@ -2122,15 +2128,15 @@
         <v>83</v>
       </c>
       <c r="J53" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B54" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C54" s="6" t="s">
         <v>5</v>
@@ -2146,15 +2152,15 @@
       <c r="H54" s="2"/>
       <c r="I54" s="2"/>
       <c r="J54" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B55" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C55" s="6" t="s">
         <v>5</v>
@@ -2170,15 +2176,15 @@
       <c r="H55" s="2"/>
       <c r="I55" s="2"/>
       <c r="J55" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B56" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C56" s="6" t="s">
         <v>5</v>
@@ -2194,15 +2200,15 @@
       <c r="H56" s="2"/>
       <c r="I56" s="2"/>
       <c r="J56" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B57" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C57" s="6" t="s">
         <v>5</v>
@@ -2222,15 +2228,15 @@
         <v>85</v>
       </c>
       <c r="J57" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B58" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C58" s="6" t="s">
         <v>5</v>
@@ -2250,15 +2256,15 @@
         <v>85</v>
       </c>
       <c r="J58" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B59" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C59" s="6" t="s">
         <v>5</v>
@@ -2278,15 +2284,15 @@
         <v>83</v>
       </c>
       <c r="J59" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B60" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C60" s="6" t="s">
         <v>5</v>
@@ -2306,15 +2312,15 @@
         <v>83</v>
       </c>
       <c r="J60" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B61" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C61" s="6" t="s">
         <v>5</v>
@@ -2330,15 +2336,15 @@
       <c r="H61" s="2"/>
       <c r="I61" s="2"/>
       <c r="J61" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B62" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C62" s="6" t="s">
         <v>5</v>
@@ -2354,15 +2360,15 @@
       <c r="H62" s="2"/>
       <c r="I62" s="2"/>
       <c r="J62" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B63" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C63" s="6" t="s">
         <v>5</v>
@@ -2378,15 +2384,15 @@
       <c r="H63" s="2"/>
       <c r="I63" s="2"/>
       <c r="J63" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B64" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C64" s="6" t="s">
         <v>5</v>
@@ -2406,15 +2412,15 @@
         <v>83</v>
       </c>
       <c r="J64" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="65" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B65" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C65" s="6" t="s">
         <v>5</v>
@@ -2434,23 +2440,25 @@
         <v>83</v>
       </c>
       <c r="J65" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="66" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B66" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C66" s="6" t="s">
         <v>80</v>
       </c>
       <c r="D66" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="E66" s="3"/>
+        <v>90</v>
+      </c>
+      <c r="E66" s="7" t="s">
+        <v>108</v>
+      </c>
       <c r="F66" s="3"/>
       <c r="G66" s="3"/>
       <c r="H66" s="3"/>
@@ -2461,18 +2469,20 @@
     </row>
     <row r="67" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B67" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C67" s="6" t="s">
         <v>80</v>
       </c>
       <c r="D67" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="E67" s="3"/>
+        <v>90</v>
+      </c>
+      <c r="E67" s="7" t="s">
+        <v>108</v>
+      </c>
       <c r="F67" s="3"/>
       <c r="G67" s="3"/>
       <c r="H67" s="3"/>
@@ -2483,18 +2493,20 @@
     </row>
     <row r="68" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B68" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C68" s="6" t="s">
         <v>80</v>
       </c>
       <c r="D68" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="E68" s="3"/>
+        <v>90</v>
+      </c>
+      <c r="E68" s="7" t="s">
+        <v>108</v>
+      </c>
       <c r="F68" s="3"/>
       <c r="G68" s="3"/>
       <c r="H68" s="3"/>
@@ -2505,18 +2517,20 @@
     </row>
     <row r="69" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B69" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C69" s="6" t="s">
         <v>80</v>
       </c>
       <c r="D69" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="E69" s="3"/>
+        <v>90</v>
+      </c>
+      <c r="E69" s="7" t="s">
+        <v>108</v>
+      </c>
       <c r="F69" s="3"/>
       <c r="G69" s="3"/>
       <c r="H69" s="3"/>
@@ -2527,18 +2541,20 @@
     </row>
     <row r="70" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B70" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C70" s="6" t="s">
         <v>80</v>
       </c>
       <c r="D70" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="E70" s="3"/>
+        <v>90</v>
+      </c>
+      <c r="E70" s="7" t="s">
+        <v>108</v>
+      </c>
       <c r="F70" s="3"/>
       <c r="G70" s="3"/>
       <c r="H70" s="3"/>
@@ -2549,18 +2565,20 @@
     </row>
     <row r="71" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B71" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C71" s="6" t="s">
         <v>80</v>
       </c>
       <c r="D71" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="E71" s="3"/>
+        <v>90</v>
+      </c>
+      <c r="E71" s="7" t="s">
+        <v>108</v>
+      </c>
       <c r="F71" s="3"/>
       <c r="G71" s="3"/>
       <c r="H71" s="3"/>
@@ -2571,18 +2589,20 @@
     </row>
     <row r="72" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B72" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C72" s="6" t="s">
         <v>80</v>
       </c>
       <c r="D72" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="E72" s="3"/>
+        <v>90</v>
+      </c>
+      <c r="E72" s="7" t="s">
+        <v>108</v>
+      </c>
       <c r="F72" s="3"/>
       <c r="G72" s="3"/>
       <c r="H72" s="3"/>
@@ -2596,15 +2616,17 @@
         <v>45</v>
       </c>
       <c r="B73" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C73" s="6" t="s">
         <v>80</v>
       </c>
       <c r="D73" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="E73" s="3"/>
+        <v>90</v>
+      </c>
+      <c r="E73" s="7" t="s">
+        <v>108</v>
+      </c>
       <c r="F73" s="3" t="s">
         <v>22</v>
       </c>
@@ -2624,15 +2646,17 @@
         <v>45</v>
       </c>
       <c r="B74" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C74" s="6" t="s">
         <v>80</v>
       </c>
       <c r="D74" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="E74" s="3"/>
+        <v>90</v>
+      </c>
+      <c r="E74" s="7" t="s">
+        <v>108</v>
+      </c>
       <c r="F74" s="3"/>
       <c r="G74" s="3"/>
       <c r="H74" s="3"/>
@@ -2646,15 +2670,17 @@
         <v>45</v>
       </c>
       <c r="B75" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C75" s="6" t="s">
         <v>80</v>
       </c>
       <c r="D75" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="E75" s="3"/>
+        <v>90</v>
+      </c>
+      <c r="E75" s="7" t="s">
+        <v>108</v>
+      </c>
       <c r="F75" s="3" t="s">
         <v>33</v>
       </c>
@@ -2674,15 +2700,17 @@
         <v>45</v>
       </c>
       <c r="B76" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C76" s="6" t="s">
         <v>80</v>
       </c>
       <c r="D76" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="E76" s="3"/>
+        <v>90</v>
+      </c>
+      <c r="E76" s="7" t="s">
+        <v>108</v>
+      </c>
       <c r="F76" s="3">
         <v>2</v>
       </c>
@@ -2702,15 +2730,17 @@
         <v>45</v>
       </c>
       <c r="B77" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C77" s="6" t="s">
         <v>80</v>
       </c>
       <c r="D77" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="E77" s="3"/>
+        <v>90</v>
+      </c>
+      <c r="E77" s="7" t="s">
+        <v>108</v>
+      </c>
       <c r="F77" s="3" t="s">
         <v>22</v>
       </c>
@@ -2730,15 +2760,17 @@
         <v>45</v>
       </c>
       <c r="B78" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C78" s="6" t="s">
         <v>80</v>
       </c>
       <c r="D78" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="E78" s="3"/>
+        <v>90</v>
+      </c>
+      <c r="E78" s="7" t="s">
+        <v>108</v>
+      </c>
       <c r="F78" s="3">
         <v>2</v>
       </c>
@@ -2758,15 +2790,17 @@
         <v>45</v>
       </c>
       <c r="B79" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C79" s="6" t="s">
         <v>80</v>
       </c>
       <c r="D79" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="E79" s="3"/>
+        <v>90</v>
+      </c>
+      <c r="E79" s="7" t="s">
+        <v>108</v>
+      </c>
       <c r="F79" s="3" t="s">
         <v>22</v>
       </c>
@@ -2786,15 +2820,17 @@
         <v>47</v>
       </c>
       <c r="B80" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C80" s="6" t="s">
         <v>80</v>
       </c>
       <c r="D80" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="E80" s="3"/>
+        <v>90</v>
+      </c>
+      <c r="E80" s="7" t="s">
+        <v>108</v>
+      </c>
       <c r="F80" s="3" t="s">
         <v>22</v>
       </c>
@@ -2814,15 +2850,17 @@
         <v>47</v>
       </c>
       <c r="B81" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C81" s="6" t="s">
         <v>80</v>
       </c>
       <c r="D81" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="E81" s="3"/>
+        <v>90</v>
+      </c>
+      <c r="E81" s="7" t="s">
+        <v>108</v>
+      </c>
       <c r="F81" s="3"/>
       <c r="G81" s="3"/>
       <c r="H81" s="3"/>
@@ -2836,15 +2874,17 @@
         <v>47</v>
       </c>
       <c r="B82" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C82" s="6" t="s">
         <v>80</v>
       </c>
       <c r="D82" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="E82" s="3"/>
+        <v>90</v>
+      </c>
+      <c r="E82" s="7" t="s">
+        <v>108</v>
+      </c>
       <c r="F82" s="3" t="s">
         <v>33</v>
       </c>
@@ -2864,15 +2904,17 @@
         <v>47</v>
       </c>
       <c r="B83" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C83" s="6" t="s">
         <v>80</v>
       </c>
       <c r="D83" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="E83" s="3"/>
+        <v>90</v>
+      </c>
+      <c r="E83" s="7" t="s">
+        <v>108</v>
+      </c>
       <c r="F83" s="3">
         <v>2</v>
       </c>
@@ -2892,15 +2934,17 @@
         <v>47</v>
       </c>
       <c r="B84" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C84" s="6" t="s">
         <v>80</v>
       </c>
       <c r="D84" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="E84" s="3"/>
+        <v>90</v>
+      </c>
+      <c r="E84" s="7" t="s">
+        <v>108</v>
+      </c>
       <c r="F84" s="3" t="s">
         <v>22</v>
       </c>
@@ -2920,15 +2964,17 @@
         <v>47</v>
       </c>
       <c r="B85" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C85" s="6" t="s">
         <v>80</v>
       </c>
       <c r="D85" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="E85" s="3"/>
+        <v>90</v>
+      </c>
+      <c r="E85" s="7" t="s">
+        <v>108</v>
+      </c>
       <c r="F85" s="3">
         <v>2</v>
       </c>
@@ -2948,15 +2994,17 @@
         <v>47</v>
       </c>
       <c r="B86" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C86" s="6" t="s">
         <v>80</v>
       </c>
       <c r="D86" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="E86" s="3"/>
+        <v>90</v>
+      </c>
+      <c r="E86" s="7" t="s">
+        <v>108</v>
+      </c>
       <c r="F86" s="3" t="s">
         <v>22</v>
       </c>
@@ -2976,15 +3024,17 @@
         <v>48</v>
       </c>
       <c r="B87" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C87" s="6" t="s">
         <v>80</v>
       </c>
       <c r="D87" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="E87" s="3"/>
+        <v>90</v>
+      </c>
+      <c r="E87" s="7" t="s">
+        <v>108</v>
+      </c>
       <c r="F87" s="3" t="s">
         <v>22</v>
       </c>
@@ -3004,15 +3054,17 @@
         <v>48</v>
       </c>
       <c r="B88" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C88" s="6" t="s">
         <v>80</v>
       </c>
       <c r="D88" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="E88" s="3"/>
+        <v>90</v>
+      </c>
+      <c r="E88" s="7" t="s">
+        <v>108</v>
+      </c>
       <c r="F88" s="3"/>
       <c r="G88" s="3"/>
       <c r="H88" s="3"/>
@@ -3026,15 +3078,17 @@
         <v>48</v>
       </c>
       <c r="B89" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C89" s="6" t="s">
         <v>80</v>
       </c>
       <c r="D89" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="E89" s="3"/>
+        <v>90</v>
+      </c>
+      <c r="E89" s="7" t="s">
+        <v>108</v>
+      </c>
       <c r="F89" s="3" t="s">
         <v>83</v>
       </c>
@@ -3054,15 +3108,17 @@
         <v>48</v>
       </c>
       <c r="B90" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C90" s="6" t="s">
         <v>80</v>
       </c>
       <c r="D90" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="E90" s="3"/>
+        <v>90</v>
+      </c>
+      <c r="E90" s="7" t="s">
+        <v>108</v>
+      </c>
       <c r="F90" s="3">
         <v>2</v>
       </c>
@@ -3082,15 +3138,17 @@
         <v>48</v>
       </c>
       <c r="B91" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C91" s="6" t="s">
         <v>80</v>
       </c>
       <c r="D91" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="E91" s="3"/>
+        <v>90</v>
+      </c>
+      <c r="E91" s="7" t="s">
+        <v>108</v>
+      </c>
       <c r="F91" s="3" t="s">
         <v>22</v>
       </c>
@@ -3110,15 +3168,17 @@
         <v>48</v>
       </c>
       <c r="B92" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C92" s="6" t="s">
         <v>80</v>
       </c>
       <c r="D92" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="E92" s="3"/>
+        <v>90</v>
+      </c>
+      <c r="E92" s="7" t="s">
+        <v>108</v>
+      </c>
       <c r="F92" s="3">
         <v>2</v>
       </c>
@@ -3138,15 +3198,17 @@
         <v>48</v>
       </c>
       <c r="B93" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C93" s="6" t="s">
         <v>80</v>
       </c>
       <c r="D93" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="E93" s="3"/>
+        <v>90</v>
+      </c>
+      <c r="E93" s="7" t="s">
+        <v>108</v>
+      </c>
       <c r="F93" s="3" t="s">
         <v>22</v>
       </c>
@@ -3166,15 +3228,17 @@
         <v>49</v>
       </c>
       <c r="B94" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C94" s="6" t="s">
         <v>80</v>
       </c>
       <c r="D94" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="E94" s="3"/>
+        <v>90</v>
+      </c>
+      <c r="E94" s="7" t="s">
+        <v>108</v>
+      </c>
       <c r="F94" s="3" t="s">
         <v>33</v>
       </c>
@@ -3194,15 +3258,17 @@
         <v>49</v>
       </c>
       <c r="B95" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C95" s="6" t="s">
         <v>80</v>
       </c>
       <c r="D95" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="E95" s="3"/>
+        <v>90</v>
+      </c>
+      <c r="E95" s="7" t="s">
+        <v>108</v>
+      </c>
       <c r="F95" s="2"/>
       <c r="G95" s="2"/>
       <c r="H95" s="2"/>
@@ -3216,15 +3282,17 @@
         <v>49</v>
       </c>
       <c r="B96" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C96" s="6" t="s">
         <v>80</v>
       </c>
       <c r="D96" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="E96" s="3"/>
+        <v>90</v>
+      </c>
+      <c r="E96" s="7" t="s">
+        <v>108</v>
+      </c>
       <c r="F96" s="2"/>
       <c r="G96" s="2"/>
       <c r="H96" s="2"/>
@@ -3238,15 +3306,17 @@
         <v>49</v>
       </c>
       <c r="B97" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C97" s="6" t="s">
         <v>80</v>
       </c>
       <c r="D97" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="E97" s="3"/>
+        <v>90</v>
+      </c>
+      <c r="E97" s="7" t="s">
+        <v>108</v>
+      </c>
       <c r="F97" s="2"/>
       <c r="G97" s="2"/>
       <c r="H97" s="2"/>
@@ -3260,15 +3330,17 @@
         <v>49</v>
       </c>
       <c r="B98" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C98" s="6" t="s">
         <v>80</v>
       </c>
       <c r="D98" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="E98" s="3"/>
+        <v>90</v>
+      </c>
+      <c r="E98" s="7" t="s">
+        <v>108</v>
+      </c>
       <c r="F98" s="3" t="s">
         <v>17</v>
       </c>
@@ -3288,15 +3360,17 @@
         <v>49</v>
       </c>
       <c r="B99" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C99" s="6" t="s">
         <v>80</v>
       </c>
       <c r="D99" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="E99" s="3"/>
+        <v>90</v>
+      </c>
+      <c r="E99" s="7" t="s">
+        <v>108</v>
+      </c>
       <c r="F99" s="3" t="s">
         <v>33</v>
       </c>
@@ -3316,15 +3390,17 @@
         <v>49</v>
       </c>
       <c r="B100" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C100" s="6" t="s">
         <v>80</v>
       </c>
       <c r="D100" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="E100" s="3"/>
+        <v>90</v>
+      </c>
+      <c r="E100" s="7" t="s">
+        <v>108</v>
+      </c>
       <c r="F100" s="3" t="s">
         <v>33</v>
       </c>
@@ -3344,15 +3420,17 @@
         <v>50</v>
       </c>
       <c r="B101" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C101" s="6" t="s">
         <v>80</v>
       </c>
       <c r="D101" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="E101" s="3"/>
+        <v>90</v>
+      </c>
+      <c r="E101" s="7" t="s">
+        <v>108</v>
+      </c>
       <c r="F101" s="3">
         <v>2</v>
       </c>
@@ -3372,15 +3450,17 @@
         <v>50</v>
       </c>
       <c r="B102" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C102" s="6" t="s">
         <v>80</v>
       </c>
       <c r="D102" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="E102" s="3"/>
+        <v>90</v>
+      </c>
+      <c r="E102" s="7" t="s">
+        <v>108</v>
+      </c>
       <c r="F102" s="2"/>
       <c r="G102" s="2"/>
       <c r="H102" s="2"/>
@@ -3394,15 +3474,17 @@
         <v>50</v>
       </c>
       <c r="B103" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C103" s="6" t="s">
         <v>80</v>
       </c>
       <c r="D103" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="E103" s="3"/>
+        <v>90</v>
+      </c>
+      <c r="E103" s="7" t="s">
+        <v>108</v>
+      </c>
       <c r="F103" s="3"/>
       <c r="G103" s="3"/>
       <c r="H103" s="3">
@@ -3420,15 +3502,17 @@
         <v>50</v>
       </c>
       <c r="B104" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C104" s="6" t="s">
         <v>80</v>
       </c>
       <c r="D104" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="E104" s="3"/>
+        <v>90</v>
+      </c>
+      <c r="E104" s="7" t="s">
+        <v>108</v>
+      </c>
       <c r="F104" s="2"/>
       <c r="G104" s="2"/>
       <c r="H104" s="2"/>
@@ -3442,15 +3526,17 @@
         <v>50</v>
       </c>
       <c r="B105" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C105" s="6" t="s">
         <v>80</v>
       </c>
       <c r="D105" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="E105" s="3"/>
+        <v>90</v>
+      </c>
+      <c r="E105" s="7" t="s">
+        <v>108</v>
+      </c>
       <c r="F105" s="2"/>
       <c r="G105" s="2"/>
       <c r="H105" s="2"/>
@@ -3464,15 +3550,17 @@
         <v>50</v>
       </c>
       <c r="B106" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C106" s="6" t="s">
         <v>80</v>
       </c>
       <c r="D106" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="E106" s="3"/>
+        <v>90</v>
+      </c>
+      <c r="E106" s="7" t="s">
+        <v>108</v>
+      </c>
       <c r="F106" s="3">
         <v>2</v>
       </c>
@@ -3492,15 +3580,17 @@
         <v>50</v>
       </c>
       <c r="B107" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C107" s="6" t="s">
         <v>80</v>
       </c>
       <c r="D107" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="E107" s="3"/>
+        <v>90</v>
+      </c>
+      <c r="E107" s="7" t="s">
+        <v>108</v>
+      </c>
       <c r="F107" s="3">
         <v>2</v>
       </c>
@@ -3520,15 +3610,17 @@
         <v>50</v>
       </c>
       <c r="B108" t="s">
-        <v>87</v>
+        <v>107</v>
       </c>
       <c r="C108" s="6" t="s">
         <v>80</v>
       </c>
       <c r="D108" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="E108" s="3"/>
+        <v>90</v>
+      </c>
+      <c r="E108" s="7" t="s">
+        <v>108</v>
+      </c>
       <c r="F108" s="2"/>
       <c r="G108" s="2"/>
       <c r="H108" s="2"/>
@@ -3539,464 +3631,506 @@
     </row>
     <row r="109" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B109" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C109" s="6" t="s">
         <v>80</v>
       </c>
       <c r="D109" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="E109" s="3"/>
+        <v>90</v>
+      </c>
+      <c r="E109" s="7" t="s">
+        <v>108</v>
+      </c>
       <c r="F109" s="2"/>
       <c r="G109" s="2"/>
       <c r="H109" s="2"/>
       <c r="I109" s="2"/>
       <c r="J109" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="110" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B110" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C110" s="6" t="s">
         <v>80</v>
       </c>
       <c r="D110" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="E110" s="3"/>
+        <v>90</v>
+      </c>
+      <c r="E110" s="7" t="s">
+        <v>108</v>
+      </c>
       <c r="F110" s="2"/>
       <c r="G110" s="2"/>
       <c r="H110" s="2"/>
       <c r="I110" s="2"/>
       <c r="J110" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="111" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B111" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C111" s="6" t="s">
         <v>80</v>
       </c>
       <c r="D111" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="E111" s="3"/>
+        <v>90</v>
+      </c>
+      <c r="E111" s="7" t="s">
+        <v>108</v>
+      </c>
       <c r="F111" s="2"/>
       <c r="G111" s="2"/>
       <c r="H111" s="2"/>
       <c r="I111" s="2"/>
       <c r="J111" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="112" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B112" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C112" s="6" t="s">
         <v>80</v>
       </c>
       <c r="D112" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="E112" s="3"/>
+        <v>90</v>
+      </c>
+      <c r="E112" s="7" t="s">
+        <v>108</v>
+      </c>
       <c r="F112" s="2"/>
       <c r="G112" s="2"/>
       <c r="H112" s="2"/>
       <c r="I112" s="2"/>
       <c r="J112" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="113" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B113" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C113" s="6" t="s">
         <v>80</v>
       </c>
       <c r="D113" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="E113" s="3"/>
+        <v>90</v>
+      </c>
+      <c r="E113" s="7" t="s">
+        <v>108</v>
+      </c>
       <c r="F113" s="2"/>
       <c r="G113" s="2"/>
       <c r="H113" s="2"/>
       <c r="I113" s="2"/>
       <c r="J113" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="114" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B114" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C114" s="6" t="s">
         <v>80</v>
       </c>
       <c r="D114" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="E114" s="3"/>
+        <v>90</v>
+      </c>
+      <c r="E114" s="7" t="s">
+        <v>108</v>
+      </c>
       <c r="F114" s="2"/>
       <c r="G114" s="2"/>
       <c r="H114" s="2"/>
       <c r="I114" s="2"/>
       <c r="J114" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="115" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B115" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C115" s="6" t="s">
         <v>80</v>
       </c>
       <c r="D115" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="E115" s="3"/>
+        <v>90</v>
+      </c>
+      <c r="E115" s="7" t="s">
+        <v>108</v>
+      </c>
       <c r="F115" s="2"/>
       <c r="G115" s="2"/>
       <c r="H115" s="2"/>
       <c r="I115" s="2"/>
       <c r="J115" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="116" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B116" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C116" s="6" t="s">
         <v>80</v>
       </c>
       <c r="D116" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="E116" s="3"/>
+        <v>90</v>
+      </c>
+      <c r="E116" s="7" t="s">
+        <v>108</v>
+      </c>
       <c r="F116" s="2"/>
       <c r="G116" s="2"/>
       <c r="H116" s="2"/>
       <c r="I116" s="2"/>
       <c r="J116" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="117" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B117" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C117" s="6" t="s">
         <v>80</v>
       </c>
       <c r="D117" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="E117" s="3"/>
+        <v>90</v>
+      </c>
+      <c r="E117" s="7" t="s">
+        <v>108</v>
+      </c>
       <c r="F117" s="2"/>
       <c r="G117" s="2"/>
       <c r="H117" s="2"/>
       <c r="I117" s="2"/>
       <c r="J117" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="118" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B118" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C118" s="6" t="s">
         <v>80</v>
       </c>
       <c r="D118" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="E118" s="3"/>
+        <v>90</v>
+      </c>
+      <c r="E118" s="7" t="s">
+        <v>108</v>
+      </c>
       <c r="F118" s="2"/>
       <c r="G118" s="2"/>
       <c r="H118" s="2"/>
       <c r="I118" s="2"/>
       <c r="J118" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="119" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B119" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C119" s="6" t="s">
         <v>80</v>
       </c>
       <c r="D119" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="E119" s="3"/>
+        <v>90</v>
+      </c>
+      <c r="E119" s="7" t="s">
+        <v>108</v>
+      </c>
       <c r="F119" s="2"/>
       <c r="G119" s="2"/>
       <c r="H119" s="2"/>
       <c r="I119" s="2"/>
       <c r="J119" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="120" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B120" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C120" s="6" t="s">
         <v>80</v>
       </c>
       <c r="D120" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="E120" s="3"/>
+        <v>90</v>
+      </c>
+      <c r="E120" s="7" t="s">
+        <v>108</v>
+      </c>
       <c r="F120" s="2"/>
       <c r="G120" s="2"/>
       <c r="H120" s="2"/>
       <c r="I120" s="2"/>
       <c r="J120" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="121" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B121" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C121" s="6" t="s">
         <v>80</v>
       </c>
       <c r="D121" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="E121" s="3"/>
+        <v>90</v>
+      </c>
+      <c r="E121" s="7" t="s">
+        <v>108</v>
+      </c>
       <c r="F121" s="2"/>
       <c r="G121" s="2"/>
       <c r="H121" s="2"/>
       <c r="I121" s="2"/>
       <c r="J121" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="122" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B122" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C122" s="6" t="s">
         <v>80</v>
       </c>
       <c r="D122" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="E122" s="3"/>
+        <v>90</v>
+      </c>
+      <c r="E122" s="7" t="s">
+        <v>108</v>
+      </c>
       <c r="F122" s="2"/>
       <c r="G122" s="2"/>
       <c r="H122" s="2"/>
       <c r="I122" s="2"/>
       <c r="J122" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="123" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B123" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C123" s="6" t="s">
         <v>80</v>
       </c>
       <c r="D123" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="E123" s="3"/>
+        <v>90</v>
+      </c>
+      <c r="E123" s="7" t="s">
+        <v>108</v>
+      </c>
       <c r="F123" s="2"/>
       <c r="G123" s="2"/>
       <c r="H123" s="2"/>
       <c r="I123" s="2"/>
       <c r="J123" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="124" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B124" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C124" s="6" t="s">
         <v>80</v>
       </c>
       <c r="D124" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="E124" s="3"/>
+        <v>90</v>
+      </c>
+      <c r="E124" s="7" t="s">
+        <v>108</v>
+      </c>
       <c r="F124" s="2"/>
       <c r="G124" s="2"/>
       <c r="H124" s="2"/>
       <c r="I124" s="2"/>
       <c r="J124" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="125" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B125" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C125" s="6" t="s">
         <v>80</v>
       </c>
       <c r="D125" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="E125" s="3"/>
+        <v>90</v>
+      </c>
+      <c r="E125" s="7" t="s">
+        <v>108</v>
+      </c>
       <c r="F125" s="2"/>
       <c r="G125" s="2"/>
       <c r="H125" s="2"/>
       <c r="I125" s="2"/>
       <c r="J125" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="126" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B126" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C126" s="6" t="s">
         <v>80</v>
       </c>
       <c r="D126" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="E126" s="3"/>
+        <v>90</v>
+      </c>
+      <c r="E126" s="7" t="s">
+        <v>108</v>
+      </c>
       <c r="F126" s="2"/>
       <c r="G126" s="2"/>
       <c r="H126" s="2"/>
       <c r="I126" s="2"/>
       <c r="J126" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="127" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B127" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C127" s="6" t="s">
         <v>80</v>
       </c>
       <c r="D127" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="E127" s="3"/>
+        <v>90</v>
+      </c>
+      <c r="E127" s="7" t="s">
+        <v>108</v>
+      </c>
       <c r="F127" s="2"/>
       <c r="G127" s="2"/>
       <c r="H127" s="2"/>
       <c r="I127" s="2"/>
       <c r="J127" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="128" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B128" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C128" s="6" t="s">
         <v>80</v>
       </c>
       <c r="D128" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="E128" s="3"/>
+        <v>90</v>
+      </c>
+      <c r="E128" s="7" t="s">
+        <v>108</v>
+      </c>
       <c r="F128" s="2"/>
       <c r="G128" s="2"/>
       <c r="H128" s="2"/>
       <c r="I128" s="2"/>
       <c r="J128" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="129" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B129" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C129" s="6" t="s">
         <v>80</v>
       </c>
       <c r="D129" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="E129" s="3"/>
+        <v>90</v>
+      </c>
+      <c r="E129" s="7" t="s">
+        <v>108</v>
+      </c>
       <c r="F129" s="2"/>
       <c r="G129" s="2"/>
       <c r="H129" s="2"/>
       <c r="I129" s="2"/>
       <c r="J129" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
   </sheetData>
@@ -4542,7 +4676,7 @@
     </row>
     <row r="34" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F34" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
   </sheetData>

</xml_diff>